<commit_message>
change excel sheet login data
</commit_message>
<xml_diff>
--- a/LoginTestCasesandData.xlsx
+++ b/LoginTestCasesandData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DAABF8-99E2-4CBD-B331-72354EC9A776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0350B345-91F3-419C-AAA8-B848A5FEC1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginTest" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>Keyword</t>
   </si>
@@ -44,12 +44,6 @@
     <t>ObjectType</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
     <t>CLICK</t>
   </si>
   <si>
@@ -71,19 +65,10 @@
     <t>Admin123</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>loginButton</t>
-  </si>
-  <si>
     <t>Inpatient Ward</t>
   </si>
   <si>
     <t>CLICKLISTHOMEPAGE</t>
-  </si>
-  <si>
-    <t>username</t>
   </si>
   <si>
     <t>Iteration1</t>
@@ -581,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +582,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -609,15 +594,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -639,16 +624,16 @@
         <v>name</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="2" t="str">
         <f>[1]Objects!$B$3</f>
@@ -675,30 +660,30 @@
         <v>name</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="2" t="str">
         <f>[1]Objects!$B$4</f>
@@ -714,7 +699,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="str">
         <f>[1]Objects!$B$5</f>
@@ -725,10 +710,10 @@
         <v>id</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -740,8 +725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E88B823-AB0D-4107-B578-734CE6DE5A43}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +740,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -767,12 +752,12 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -784,26 +769,30 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>4</v>
+      <c r="C3" s="2" t="str">
+        <f>[1]Objects!$B$2</f>
+        <v>username</v>
+      </c>
+      <c r="D3" s="2" t="str">
+        <f>[1]Objects!$C$2</f>
+        <v>name</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>[1]Objects!$B$3</f>
+        <v>password</v>
+      </c>
+      <c r="D4" s="2" t="str">
+        <f>[1]Objects!$C$3</f>
+        <v>name</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -812,53 +801,53 @@
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>4</v>
+      <c r="C5" s="2" t="str">
+        <f>[1]Objects!$B$3</f>
+        <v>password</v>
+      </c>
+      <c r="D5" s="2" t="str">
+        <f>[1]Objects!$C$3</f>
+        <v>name</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f>[1]Objects!$B$4</f>
+        <v>loginButton</v>
+      </c>
+      <c r="D7" s="2" t="str">
+        <f>[1]Objects!$C$4</f>
+        <v>id</v>
       </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>